<commit_message>
inventory pageobjects file added
</commit_message>
<xml_diff>
--- a/src/com/eprint/testData/Estimates/SheetFedDigital-SingleItem.xlsx
+++ b/src/com/eprint/testData/Estimates/SheetFedDigital-SingleItem.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1580" uniqueCount="526">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1580" uniqueCount="528">
   <si>
     <t>Company</t>
   </si>
@@ -1601,13 +1601,19 @@
   </si>
   <si>
     <t>Blup89</t>
+  </si>
+  <si>
+    <t>SWL</t>
+  </si>
+  <si>
+    <t>Estimates Add – Sheet Fed Digital - Single Item- Price For Whole Pack - Double Sided Black and White and Colour - Digital Press Type Speed Weight Lookup</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1652,6 +1658,12 @@
     <font>
       <b/>
       <sz val="14"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -1772,7 +1784,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -1821,6 +1833,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -3018,26 +3033,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="I61" sqref="I61"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="23.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="26.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="31.42578125" customWidth="1"/>
+    <col min="6" max="6" width="62.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18">
-      <c r="A1" s="32" t="s">
-        <v>473</v>
-      </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
+    <row r="1" spans="1:6">
+      <c r="A1" s="36" t="s">
+        <v>527</v>
+      </c>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="2" t="s">
@@ -3173,7 +3188,7 @@
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
     </row>
-    <row r="15" spans="1:6" ht="15.75" thickBot="1">
+    <row r="15" spans="1:6">
       <c r="A15" s="2" t="s">
         <v>15</v>
       </c>
@@ -3185,12 +3200,12 @@
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
     </row>
-    <row r="16" spans="1:6" ht="15.75" thickTop="1">
+    <row r="16" spans="1:6">
       <c r="A16" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="27" t="s">
-        <v>476</v>
+      <c r="B16" s="3" t="s">
+        <v>526</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
@@ -3909,6 +3924,7 @@
     <hyperlink ref="B33" r:id="rId1" location="'Digital Press'!A1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
19-4-14 office eve . completed sfd swl scripts and data
</commit_message>
<xml_diff>
--- a/src/com/eprint/testData/Estimates/SheetFedDigital-SingleItem.xlsx
+++ b/src/com/eprint/testData/Estimates/SheetFedDigital-SingleItem.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="9615" windowHeight="7935" tabRatio="872" firstSheet="13" activeTab="15"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="9615" windowHeight="7935" tabRatio="467" firstSheet="24" activeTab="24"/>
   </bookViews>
   <sheets>
     <sheet name="Paper Stock Supplied" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3950" uniqueCount="844">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3950" uniqueCount="1160">
   <si>
     <t>Company</t>
   </si>
@@ -2570,13 +2570,961 @@
   </si>
   <si>
     <t>$32.16</t>
+  </si>
+  <si>
+    <t>$42.40</t>
+  </si>
+  <si>
+    <t>$48.96</t>
+  </si>
+  <si>
+    <t>$1.15</t>
+  </si>
+  <si>
+    <t>$50.11</t>
+  </si>
+  <si>
+    <t>12.53</t>
+  </si>
+  <si>
+    <t>62.64</t>
+  </si>
+  <si>
+    <t>$13.68</t>
+  </si>
+  <si>
+    <t>$47.50</t>
+  </si>
+  <si>
+    <t>$53.96</t>
+  </si>
+  <si>
+    <t>$1.25</t>
+  </si>
+  <si>
+    <t>$55.21</t>
+  </si>
+  <si>
+    <t>13.80</t>
+  </si>
+  <si>
+    <t>69.02</t>
+  </si>
+  <si>
+    <t>(21.81%)</t>
+  </si>
+  <si>
+    <t>$76.45</t>
+  </si>
+  <si>
+    <t>$82.35</t>
+  </si>
+  <si>
+    <t>$84.16</t>
+  </si>
+  <si>
+    <t>21.04</t>
+  </si>
+  <si>
+    <t>105.20</t>
+  </si>
+  <si>
+    <t>$42.85</t>
+  </si>
+  <si>
+    <t>$49.41</t>
+  </si>
+  <si>
+    <t>$1.16</t>
+  </si>
+  <si>
+    <t>$50.56</t>
+  </si>
+  <si>
+    <t>12.64</t>
+  </si>
+  <si>
+    <t>63.20</t>
+  </si>
+  <si>
+    <t>SWL 3d Stickers</t>
+  </si>
+  <si>
+    <t>$6.26</t>
+  </si>
+  <si>
+    <t>$68.90</t>
+  </si>
+  <si>
+    <t>$6.90</t>
+  </si>
+  <si>
+    <t>$75.92</t>
+  </si>
+  <si>
+    <t>$15.06</t>
+  </si>
+  <si>
+    <t>$10.52</t>
+  </si>
+  <si>
+    <t>$115.72</t>
+  </si>
+  <si>
+    <t>$22.85</t>
+  </si>
+  <si>
+    <t>(21.72%)</t>
+  </si>
+  <si>
+    <t>$69.52</t>
+  </si>
+  <si>
+    <t>SWL T Shirt Prints</t>
+  </si>
+  <si>
+    <t>$44.20</t>
+  </si>
+  <si>
+    <t>$1.05</t>
+  </si>
+  <si>
+    <t>$45.25</t>
+  </si>
+  <si>
+    <t>11.31</t>
+  </si>
+  <si>
+    <t>56.57</t>
+  </si>
+  <si>
+    <t>$5.66</t>
+  </si>
+  <si>
+    <t>$62.23</t>
+  </si>
+  <si>
+    <t>$12.37</t>
+  </si>
+  <si>
+    <t>(21.87%)</t>
+  </si>
+  <si>
+    <t>$41.88</t>
+  </si>
+  <si>
+    <t>$48.45</t>
+  </si>
+  <si>
+    <t>$1.14</t>
+  </si>
+  <si>
+    <t>$49.59</t>
+  </si>
+  <si>
+    <t>12.40</t>
+  </si>
+  <si>
+    <t>61.98</t>
+  </si>
+  <si>
+    <t>$6.20</t>
+  </si>
+  <si>
+    <t>$68.18</t>
+  </si>
+  <si>
+    <t>$13.53</t>
+  </si>
+  <si>
+    <t>$66.48</t>
+  </si>
+  <si>
+    <t>$72.58</t>
+  </si>
+  <si>
+    <t>$74.19</t>
+  </si>
+  <si>
+    <t>18.55</t>
+  </si>
+  <si>
+    <t>92.74</t>
+  </si>
+  <si>
+    <t>$9.27</t>
+  </si>
+  <si>
+    <t>$102.01</t>
+  </si>
+  <si>
+    <t>$20.16</t>
+  </si>
+  <si>
+    <t>$37.92</t>
+  </si>
+  <si>
+    <t>$44.58</t>
+  </si>
+  <si>
+    <t>$1.06</t>
+  </si>
+  <si>
+    <t>$45.63</t>
+  </si>
+  <si>
+    <t>11.41</t>
+  </si>
+  <si>
+    <t>57.04</t>
+  </si>
+  <si>
+    <t>$5.70</t>
+  </si>
+  <si>
+    <t>$62.74</t>
+  </si>
+  <si>
+    <t>$12.46</t>
+  </si>
+  <si>
+    <t>(21.85%)</t>
+  </si>
+  <si>
+    <t>$1.62</t>
+  </si>
+  <si>
+    <t>SWL Canvas Prints</t>
+  </si>
+  <si>
+    <t>Cv154</t>
+  </si>
+  <si>
+    <t>52</t>
+  </si>
+  <si>
+    <t>$14.08</t>
+  </si>
+  <si>
+    <t>$15.83</t>
+  </si>
+  <si>
+    <t>$17.14</t>
+  </si>
+  <si>
+    <t>$16.27</t>
+  </si>
+  <si>
+    <t>$21.20</t>
+  </si>
+  <si>
+    <t>$21.79</t>
+  </si>
+  <si>
+    <t>5.45</t>
+  </si>
+  <si>
+    <t>27.24</t>
+  </si>
+  <si>
+    <t>$2.72</t>
+  </si>
+  <si>
+    <t>$29.96</t>
+  </si>
+  <si>
+    <t>$6.04</t>
+  </si>
+  <si>
+    <t>(22.17%)</t>
+  </si>
+  <si>
+    <t>$22.91</t>
+  </si>
+  <si>
+    <t>$23.54</t>
+  </si>
+  <si>
+    <t>5.89</t>
+  </si>
+  <si>
+    <t>29.43</t>
+  </si>
+  <si>
+    <t>$2.94</t>
+  </si>
+  <si>
+    <t>$32.37</t>
+  </si>
+  <si>
+    <t>$6.52</t>
+  </si>
+  <si>
+    <t>(22.14%)</t>
+  </si>
+  <si>
+    <t>$24.20</t>
+  </si>
+  <si>
+    <t>$24.85</t>
+  </si>
+  <si>
+    <t>6.21</t>
+  </si>
+  <si>
+    <t>31.07</t>
+  </si>
+  <si>
+    <t>$3.11</t>
+  </si>
+  <si>
+    <t>$34.18</t>
+  </si>
+  <si>
+    <t>$23.34</t>
+  </si>
+  <si>
+    <t>$23.98</t>
+  </si>
+  <si>
+    <t>29.97</t>
+  </si>
+  <si>
+    <t>$32.97</t>
+  </si>
+  <si>
+    <t>$0.65</t>
+  </si>
+  <si>
+    <t>SWL 3D Banner</t>
+  </si>
+  <si>
+    <t>55</t>
+  </si>
+  <si>
+    <t>66</t>
+  </si>
+  <si>
+    <t>88</t>
+  </si>
+  <si>
+    <t>99</t>
+  </si>
+  <si>
+    <t>$15.95</t>
+  </si>
+  <si>
+    <t>$23.03</t>
+  </si>
+  <si>
+    <t>$23.66</t>
+  </si>
+  <si>
+    <t>29.58</t>
+  </si>
+  <si>
+    <t>$2.96</t>
+  </si>
+  <si>
+    <t>$32.54</t>
+  </si>
+  <si>
+    <t>$6.55</t>
+  </si>
+  <si>
+    <t>$17.82</t>
+  </si>
+  <si>
+    <t>$24.87</t>
+  </si>
+  <si>
+    <t>$0.67</t>
+  </si>
+  <si>
+    <t>$25.53</t>
+  </si>
+  <si>
+    <t>6.38</t>
+  </si>
+  <si>
+    <t>5.92</t>
+  </si>
+  <si>
+    <t>31.92</t>
+  </si>
+  <si>
+    <t>$3.19</t>
+  </si>
+  <si>
+    <t>$35.11</t>
+  </si>
+  <si>
+    <t>$7.05</t>
+  </si>
+  <si>
+    <t>(22.10%)</t>
+  </si>
+  <si>
+    <t>$18.84</t>
+  </si>
+  <si>
+    <t>$25.87</t>
+  </si>
+  <si>
+    <t>$0.69</t>
+  </si>
+  <si>
+    <t>$26.55</t>
+  </si>
+  <si>
+    <t>6.64</t>
+  </si>
+  <si>
+    <t>33.19</t>
+  </si>
+  <si>
+    <t>$3.32</t>
+  </si>
+  <si>
+    <t>$36.51</t>
+  </si>
+  <si>
+    <t>$7.32</t>
+  </si>
+  <si>
+    <t>61</t>
+  </si>
+  <si>
+    <t>43</t>
+  </si>
+  <si>
+    <t>$20.00</t>
+  </si>
+  <si>
+    <t>$27.00</t>
+  </si>
+  <si>
+    <t>$0.71</t>
+  </si>
+  <si>
+    <t>$27.71</t>
+  </si>
+  <si>
+    <t>6.93</t>
+  </si>
+  <si>
+    <t>34.64</t>
+  </si>
+  <si>
+    <t>$3.46</t>
+  </si>
+  <si>
+    <t>$38.10</t>
+  </si>
+  <si>
+    <t>$7.64</t>
+  </si>
+  <si>
+    <t>$18.16</t>
+  </si>
+  <si>
+    <t>$25.20</t>
+  </si>
+  <si>
+    <t>6.47</t>
+  </si>
+  <si>
+    <t>32.34</t>
+  </si>
+  <si>
+    <t>$3.23</t>
+  </si>
+  <si>
+    <t>$35.57</t>
+  </si>
+  <si>
+    <t>$16.73</t>
+  </si>
+  <si>
+    <t>$23.80</t>
+  </si>
+  <si>
+    <t>$24.44</t>
+  </si>
+  <si>
+    <t>6.11</t>
+  </si>
+  <si>
+    <t>30.56</t>
+  </si>
+  <si>
+    <t>$3.06</t>
+  </si>
+  <si>
+    <t>$33.62</t>
+  </si>
+  <si>
+    <t>$6.76</t>
+  </si>
+  <si>
+    <t>$14.69</t>
+  </si>
+  <si>
+    <t>$21.80</t>
+  </si>
+  <si>
+    <t>$22.40</t>
+  </si>
+  <si>
+    <t>5.60</t>
+  </si>
+  <si>
+    <t>28.01</t>
+  </si>
+  <si>
+    <t>$2.80</t>
+  </si>
+  <si>
+    <t>$30.81</t>
+  </si>
+  <si>
+    <t>$6.21</t>
+  </si>
+  <si>
+    <t>SWL Advertisement</t>
+  </si>
+  <si>
+    <t>Adv897</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>62</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>SWL SheetMouldCovers</t>
+  </si>
+  <si>
+    <t>SM Covers23</t>
+  </si>
+  <si>
+    <t>$11.79</t>
+  </si>
+  <si>
+    <t>$18.95</t>
+  </si>
+  <si>
+    <t>$19.50</t>
+  </si>
+  <si>
+    <t>24.37</t>
+  </si>
+  <si>
+    <t>(22.24%)</t>
+  </si>
+  <si>
+    <t>$12.04</t>
+  </si>
+  <si>
+    <t>$19.20</t>
+  </si>
+  <si>
+    <t>$19.75</t>
+  </si>
+  <si>
+    <t>4.94</t>
+  </si>
+  <si>
+    <t>24.69</t>
+  </si>
+  <si>
+    <t>$18.42</t>
+  </si>
+  <si>
+    <t>$25.45</t>
+  </si>
+  <si>
+    <t>$0.68</t>
+  </si>
+  <si>
+    <t>$26.13</t>
+  </si>
+  <si>
+    <t>6.53</t>
+  </si>
+  <si>
+    <t>32.66</t>
+  </si>
+  <si>
+    <t>$7.21</t>
+  </si>
+  <si>
+    <t>$2.44</t>
+  </si>
+  <si>
+    <t>$26.81</t>
+  </si>
+  <si>
+    <t>$2.47</t>
+  </si>
+  <si>
+    <t>$27.16</t>
+  </si>
+  <si>
+    <t>$3.27</t>
+  </si>
+  <si>
+    <t>$35.93</t>
+  </si>
+  <si>
+    <t>SWL Pad Prints</t>
+  </si>
+  <si>
+    <t>PP425</t>
+  </si>
+  <si>
+    <t>39</t>
+  </si>
+  <si>
+    <t>71</t>
+  </si>
+  <si>
+    <t>28</t>
+  </si>
+  <si>
+    <t>$19.40</t>
+  </si>
+  <si>
+    <t>$26.41</t>
+  </si>
+  <si>
+    <t>$27.11</t>
+  </si>
+  <si>
+    <t>6.78</t>
+  </si>
+  <si>
+    <t>33.89</t>
+  </si>
+  <si>
+    <t>$3.39</t>
+  </si>
+  <si>
+    <t>$37.28</t>
+  </si>
+  <si>
+    <t>$7.48</t>
+  </si>
+  <si>
+    <t>$14.59</t>
+  </si>
+  <si>
+    <t>$21.70</t>
+  </si>
+  <si>
+    <t>$22.30</t>
+  </si>
+  <si>
+    <t>5.58</t>
+  </si>
+  <si>
+    <t>27.88</t>
+  </si>
+  <si>
+    <t>$2.79</t>
+  </si>
+  <si>
+    <t>$30.67</t>
+  </si>
+  <si>
+    <t>$6.18</t>
+  </si>
+  <si>
+    <t>$18.31</t>
+  </si>
+  <si>
+    <t>$25.34</t>
+  </si>
+  <si>
+    <t>$26.02</t>
+  </si>
+  <si>
+    <t>6.50</t>
+  </si>
+  <si>
+    <t>32.52</t>
+  </si>
+  <si>
+    <t>$3.25</t>
+  </si>
+  <si>
+    <t>$35.77</t>
+  </si>
+  <si>
+    <t>$7.18</t>
+  </si>
+  <si>
+    <t>(22.07%)</t>
+  </si>
+  <si>
+    <t>$13.50</t>
+  </si>
+  <si>
+    <t>$20.63</t>
+  </si>
+  <si>
+    <t>$21.21</t>
+  </si>
+  <si>
+    <t>26.51</t>
+  </si>
+  <si>
+    <t>$29.16</t>
+  </si>
+  <si>
+    <t>SWL Posters</t>
+  </si>
+  <si>
+    <t>Posters 2332</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>75</t>
+  </si>
+  <si>
+    <t>$12.70</t>
+  </si>
+  <si>
+    <t>$19.85</t>
+  </si>
+  <si>
+    <t>$20.41</t>
+  </si>
+  <si>
+    <t>5.10</t>
+  </si>
+  <si>
+    <t>25.52</t>
+  </si>
+  <si>
+    <t>$2.55</t>
+  </si>
+  <si>
+    <t>$28.07</t>
+  </si>
+  <si>
+    <t>$5.67</t>
+  </si>
+  <si>
+    <t>(22.23%)</t>
+  </si>
+  <si>
+    <t>$13.00</t>
+  </si>
+  <si>
+    <t>$20.14</t>
+  </si>
+  <si>
+    <t>$20.71</t>
+  </si>
+  <si>
+    <t>5.18</t>
+  </si>
+  <si>
+    <t>25.89</t>
+  </si>
+  <si>
+    <t>$2.59</t>
+  </si>
+  <si>
+    <t>$28.48</t>
+  </si>
+  <si>
+    <t>$5.75</t>
+  </si>
+  <si>
+    <t>(22.20%)</t>
+  </si>
+  <si>
+    <t>$16.90</t>
+  </si>
+  <si>
+    <t>$24.61</t>
+  </si>
+  <si>
+    <t>6.15</t>
+  </si>
+  <si>
+    <t>30.77</t>
+  </si>
+  <si>
+    <t>$3.08</t>
+  </si>
+  <si>
+    <t>$6.81</t>
+  </si>
+  <si>
+    <t>$22.00</t>
+  </si>
+  <si>
+    <t>$28.96</t>
+  </si>
+  <si>
+    <t>$0.75</t>
+  </si>
+  <si>
+    <t>$29.71</t>
+  </si>
+  <si>
+    <t>7.43</t>
+  </si>
+  <si>
+    <t>37.14</t>
+  </si>
+  <si>
+    <t>$3.71</t>
+  </si>
+  <si>
+    <t>$40.85</t>
+  </si>
+  <si>
+    <t>$8.18</t>
+  </si>
+  <si>
+    <t>$33.85</t>
+  </si>
+  <si>
+    <t>SWL Flyers</t>
+  </si>
+  <si>
+    <t>Flyers38799</t>
+  </si>
+  <si>
+    <t>$83.44</t>
+  </si>
+  <si>
+    <t>$90.40</t>
+  </si>
+  <si>
+    <t>$1.96</t>
+  </si>
+  <si>
+    <t>$92.36</t>
+  </si>
+  <si>
+    <t>23.09</t>
+  </si>
+  <si>
+    <t>115.46</t>
+  </si>
+  <si>
+    <t>$11.55</t>
+  </si>
+  <si>
+    <t>$127.01</t>
+  </si>
+  <si>
+    <t>$25.06</t>
+  </si>
+  <si>
+    <t>(21.70%)</t>
+  </si>
+  <si>
+    <t>$95.00</t>
+  </si>
+  <si>
+    <t>$101.73</t>
+  </si>
+  <si>
+    <t>$2.19</t>
+  </si>
+  <si>
+    <t>$103.92</t>
+  </si>
+  <si>
+    <t>25.98</t>
+  </si>
+  <si>
+    <t>129.91</t>
+  </si>
+  <si>
+    <t>$12.99</t>
+  </si>
+  <si>
+    <t>$142.90</t>
+  </si>
+  <si>
+    <t>$28.18</t>
+  </si>
+  <si>
+    <t>$160.62</t>
+  </si>
+  <si>
+    <t>$167.27</t>
+  </si>
+  <si>
+    <t>$3.49</t>
+  </si>
+  <si>
+    <t>$170.76</t>
+  </si>
+  <si>
+    <t>42.69</t>
+  </si>
+  <si>
+    <t>213.45</t>
+  </si>
+  <si>
+    <t>$21.35</t>
+  </si>
+  <si>
+    <t>$234.80</t>
+  </si>
+  <si>
+    <t>$46.18</t>
+  </si>
+  <si>
+    <t>(21.64%)</t>
+  </si>
+  <si>
+    <t>$84.46</t>
+  </si>
+  <si>
+    <t>$91.40</t>
+  </si>
+  <si>
+    <t>$1.98</t>
+  </si>
+  <si>
+    <t>$93.38</t>
+  </si>
+  <si>
+    <t>23.35</t>
+  </si>
+  <si>
+    <t>116.73</t>
+  </si>
+  <si>
+    <t>$11.67</t>
+  </si>
+  <si>
+    <t>$128.40</t>
+  </si>
+  <si>
+    <t>$25.33</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2643,6 +3591,14 @@
       <u/>
       <sz val="10"/>
       <color theme="3" tint="0.39997558519241921"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -2763,7 +3719,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -2810,6 +3766,7 @@
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3137,14 +4094,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="39" t="s">
         <v>240</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="2" t="s">
@@ -4033,14 +4990,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="43" t="s">
         <v>538</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="2" t="s">
@@ -4305,14 +5262,14 @@
       <c r="F26" s="1"/>
     </row>
     <row r="29" spans="1:6">
-      <c r="A29" s="39" t="s">
+      <c r="A29" s="40" t="s">
         <v>475</v>
       </c>
-      <c r="B29" s="40"/>
-      <c r="C29" s="40"/>
-      <c r="D29" s="40"/>
-      <c r="E29" s="40"/>
-      <c r="F29" s="41"/>
+      <c r="B29" s="41"/>
+      <c r="C29" s="41"/>
+      <c r="D29" s="41"/>
+      <c r="E29" s="41"/>
+      <c r="F29" s="42"/>
     </row>
     <row r="30" spans="1:6">
       <c r="A30" s="7" t="s">
@@ -4934,14 +5891,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="43" t="s">
         <v>537</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="2" t="s">
@@ -5206,14 +6163,14 @@
       <c r="F26" s="1"/>
     </row>
     <row r="29" spans="1:6">
-      <c r="A29" s="39" t="s">
+      <c r="A29" s="40" t="s">
         <v>475</v>
       </c>
-      <c r="B29" s="40"/>
-      <c r="C29" s="40"/>
-      <c r="D29" s="40"/>
-      <c r="E29" s="40"/>
-      <c r="F29" s="41"/>
+      <c r="B29" s="41"/>
+      <c r="C29" s="41"/>
+      <c r="D29" s="41"/>
+      <c r="E29" s="41"/>
+      <c r="F29" s="42"/>
     </row>
     <row r="30" spans="1:6">
       <c r="A30" s="7" t="s">
@@ -5834,14 +6791,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="43" t="s">
         <v>539</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="2" t="s">
@@ -6106,14 +7063,14 @@
       <c r="F26" s="1"/>
     </row>
     <row r="29" spans="1:6">
-      <c r="A29" s="39" t="s">
+      <c r="A29" s="40" t="s">
         <v>475</v>
       </c>
-      <c r="B29" s="40"/>
-      <c r="C29" s="40"/>
-      <c r="D29" s="40"/>
-      <c r="E29" s="40"/>
-      <c r="F29" s="41"/>
+      <c r="B29" s="41"/>
+      <c r="C29" s="41"/>
+      <c r="D29" s="41"/>
+      <c r="E29" s="41"/>
+      <c r="F29" s="42"/>
     </row>
     <row r="30" spans="1:6">
       <c r="A30" s="7" t="s">
@@ -6734,14 +7691,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="43" t="s">
         <v>540</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="2" t="s">
@@ -7006,14 +7963,14 @@
       <c r="F26" s="1"/>
     </row>
     <row r="29" spans="1:6">
-      <c r="A29" s="39" t="s">
+      <c r="A29" s="40" t="s">
         <v>475</v>
       </c>
-      <c r="B29" s="40"/>
-      <c r="C29" s="40"/>
-      <c r="D29" s="40"/>
-      <c r="E29" s="40"/>
-      <c r="F29" s="41"/>
+      <c r="B29" s="41"/>
+      <c r="C29" s="41"/>
+      <c r="D29" s="41"/>
+      <c r="E29" s="41"/>
+      <c r="F29" s="42"/>
     </row>
     <row r="30" spans="1:6">
       <c r="A30" s="7" t="s">
@@ -7635,14 +8592,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="43" t="s">
         <v>541</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="2" t="s">
@@ -7907,14 +8864,14 @@
       <c r="F26" s="1"/>
     </row>
     <row r="29" spans="1:6">
-      <c r="A29" s="39" t="s">
+      <c r="A29" s="40" t="s">
         <v>475</v>
       </c>
-      <c r="B29" s="40"/>
-      <c r="C29" s="40"/>
-      <c r="D29" s="40"/>
-      <c r="E29" s="40"/>
-      <c r="F29" s="41"/>
+      <c r="B29" s="41"/>
+      <c r="C29" s="41"/>
+      <c r="D29" s="41"/>
+      <c r="E29" s="41"/>
+      <c r="F29" s="42"/>
     </row>
     <row r="30" spans="1:6">
       <c r="A30" s="7" t="s">
@@ -8535,14 +9492,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="43" t="s">
         <v>542</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="2" t="s">
@@ -8807,14 +9764,14 @@
       <c r="F26" s="1"/>
     </row>
     <row r="29" spans="1:6">
-      <c r="A29" s="39" t="s">
+      <c r="A29" s="40" t="s">
         <v>475</v>
       </c>
-      <c r="B29" s="40"/>
-      <c r="C29" s="40"/>
-      <c r="D29" s="40"/>
-      <c r="E29" s="40"/>
-      <c r="F29" s="41"/>
+      <c r="B29" s="41"/>
+      <c r="C29" s="41"/>
+      <c r="D29" s="41"/>
+      <c r="E29" s="41"/>
+      <c r="F29" s="42"/>
     </row>
     <row r="30" spans="1:6">
       <c r="A30" s="7" t="s">
@@ -9422,7 +10379,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D52" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="F61" sqref="F61"/>
     </sheetView>
   </sheetViews>
@@ -9435,14 +10392,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="43" t="s">
         <v>543</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="2" t="s">
@@ -9707,14 +10664,14 @@
       <c r="F26" s="1"/>
     </row>
     <row r="29" spans="1:6">
-      <c r="A29" s="39" t="s">
+      <c r="A29" s="40" t="s">
         <v>475</v>
       </c>
-      <c r="B29" s="40"/>
-      <c r="C29" s="40"/>
-      <c r="D29" s="40"/>
-      <c r="E29" s="40"/>
-      <c r="F29" s="41"/>
+      <c r="B29" s="41"/>
+      <c r="C29" s="41"/>
+      <c r="D29" s="41"/>
+      <c r="E29" s="41"/>
+      <c r="F29" s="42"/>
     </row>
     <row r="30" spans="1:6">
       <c r="A30" s="7" t="s">
@@ -10322,8 +11279,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F68"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="F39" sqref="B39:F40"/>
+    <sheetView topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -10335,14 +11292,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="43" t="s">
         <v>544</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="2" t="s">
@@ -10495,7 +11452,7 @@
         <v>17</v>
       </c>
       <c r="B16" s="32" t="s">
-        <v>527</v>
+        <v>869</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
@@ -10607,21 +11564,21 @@
       <c r="F26" s="1"/>
     </row>
     <row r="29" spans="1:6">
-      <c r="A29" s="39" t="s">
+      <c r="A29" s="40" t="s">
         <v>475</v>
       </c>
-      <c r="B29" s="40"/>
-      <c r="C29" s="40"/>
-      <c r="D29" s="40"/>
-      <c r="E29" s="40"/>
-      <c r="F29" s="41"/>
+      <c r="B29" s="41"/>
+      <c r="C29" s="41"/>
+      <c r="D29" s="41"/>
+      <c r="E29" s="41"/>
+      <c r="F29" s="42"/>
     </row>
     <row r="30" spans="1:6">
       <c r="A30" s="7" t="s">
         <v>32</v>
       </c>
       <c r="B30" s="32" t="s">
-        <v>527</v>
+        <v>869</v>
       </c>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
@@ -10717,7 +11674,7 @@
         <v>51</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>52</v>
+        <v>244</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>53</v>
@@ -10914,16 +11871,16 @@
       </c>
       <c r="B52" s="12"/>
       <c r="C52" s="1" t="s">
-        <v>483</v>
+        <v>198</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>484</v>
+        <v>198</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>485</v>
-      </c>
-      <c r="F52" s="8" t="s">
-        <v>483</v>
+        <v>198</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>198</v>
       </c>
     </row>
     <row r="53" spans="1:6">
@@ -10932,16 +11889,16 @@
       </c>
       <c r="B53" s="12"/>
       <c r="C53" s="1" t="s">
-        <v>486</v>
+        <v>844</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>487</v>
+        <v>851</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>488</v>
+        <v>858</v>
       </c>
       <c r="F53" s="8" t="s">
-        <v>489</v>
+        <v>863</v>
       </c>
     </row>
     <row r="54" spans="1:6">
@@ -10968,16 +11925,16 @@
       </c>
       <c r="B55" s="12"/>
       <c r="C55" s="1" t="s">
-        <v>490</v>
+        <v>845</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>491</v>
+        <v>852</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>492</v>
+        <v>859</v>
       </c>
       <c r="F55" s="8" t="s">
-        <v>493</v>
+        <v>864</v>
       </c>
     </row>
     <row r="56" spans="1:6">
@@ -10986,16 +11943,16 @@
       </c>
       <c r="B56" s="12"/>
       <c r="C56" s="1" t="s">
-        <v>494</v>
+        <v>846</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>495</v>
+        <v>853</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>496</v>
+        <v>87</v>
       </c>
       <c r="F56" s="8" t="s">
-        <v>494</v>
+        <v>865</v>
       </c>
     </row>
     <row r="57" spans="1:6">
@@ -11004,16 +11961,16 @@
       </c>
       <c r="B57" s="12"/>
       <c r="C57" s="1" t="s">
-        <v>497</v>
+        <v>847</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>498</v>
+        <v>854</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>499</v>
+        <v>860</v>
       </c>
       <c r="F57" s="8" t="s">
-        <v>500</v>
+        <v>866</v>
       </c>
     </row>
     <row r="58" spans="1:6">
@@ -11040,16 +11997,16 @@
       </c>
       <c r="B59" s="12"/>
       <c r="C59" s="1" t="s">
-        <v>501</v>
+        <v>848</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>502</v>
+        <v>855</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>503</v>
+        <v>861</v>
       </c>
       <c r="F59" s="8" t="s">
-        <v>504</v>
+        <v>867</v>
       </c>
     </row>
     <row r="60" spans="1:6">
@@ -11058,16 +12015,16 @@
       </c>
       <c r="B60" s="12"/>
       <c r="C60" s="1" t="s">
-        <v>505</v>
+        <v>849</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>506</v>
+        <v>856</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>507</v>
+        <v>862</v>
       </c>
       <c r="F60" s="8" t="s">
-        <v>508</v>
+        <v>868</v>
       </c>
     </row>
     <row r="61" spans="1:6">
@@ -11078,16 +12035,16 @@
         <v>115</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>509</v>
+        <v>870</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>510</v>
+        <v>872</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>511</v>
+        <v>875</v>
       </c>
       <c r="F61" s="8" t="s">
-        <v>512</v>
+        <v>607</v>
       </c>
     </row>
     <row r="62" spans="1:6">
@@ -11096,16 +12053,16 @@
       </c>
       <c r="B62" s="12"/>
       <c r="C62" s="1" t="s">
-        <v>513</v>
+        <v>871</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>514</v>
+        <v>873</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>515</v>
+        <v>876</v>
       </c>
       <c r="F62" s="8" t="s">
-        <v>516</v>
+        <v>879</v>
       </c>
     </row>
     <row r="63" spans="1:6">
@@ -11114,16 +12071,16 @@
       </c>
       <c r="B63" s="12"/>
       <c r="C63" s="1" t="s">
-        <v>517</v>
+        <v>850</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>518</v>
+        <v>874</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>519</v>
+        <v>877</v>
       </c>
       <c r="F63" s="8" t="s">
-        <v>520</v>
+        <v>661</v>
       </c>
     </row>
     <row r="64" spans="1:6">
@@ -11132,16 +12089,16 @@
       </c>
       <c r="B64" s="12"/>
       <c r="C64" s="1" t="s">
-        <v>521</v>
+        <v>469</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>522</v>
+        <v>857</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>523</v>
+        <v>878</v>
       </c>
       <c r="F64" s="8" t="s">
-        <v>524</v>
+        <v>469</v>
       </c>
     </row>
     <row r="65" spans="1:6">
@@ -11222,8 +12179,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F68"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="F39" sqref="B39:F40"/>
+    <sheetView topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -11235,14 +12192,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="43" t="s">
         <v>545</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="2" t="s">
@@ -11395,7 +12352,7 @@
         <v>17</v>
       </c>
       <c r="B16" s="32" t="s">
-        <v>527</v>
+        <v>880</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
@@ -11507,21 +12464,21 @@
       <c r="F26" s="1"/>
     </row>
     <row r="29" spans="1:6">
-      <c r="A29" s="39" t="s">
+      <c r="A29" s="40" t="s">
         <v>475</v>
       </c>
-      <c r="B29" s="40"/>
-      <c r="C29" s="40"/>
-      <c r="D29" s="40"/>
-      <c r="E29" s="40"/>
-      <c r="F29" s="41"/>
+      <c r="B29" s="41"/>
+      <c r="C29" s="41"/>
+      <c r="D29" s="41"/>
+      <c r="E29" s="41"/>
+      <c r="F29" s="42"/>
     </row>
     <row r="30" spans="1:6">
       <c r="A30" s="7" t="s">
         <v>32</v>
       </c>
       <c r="B30" s="32" t="s">
-        <v>527</v>
+        <v>880</v>
       </c>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
@@ -11617,7 +12574,7 @@
         <v>51</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>52</v>
+        <v>244</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>53</v>
@@ -11814,16 +12771,16 @@
       </c>
       <c r="B52" s="12"/>
       <c r="C52" s="1" t="s">
-        <v>483</v>
+        <v>198</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>484</v>
+        <v>198</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>485</v>
+        <v>198</v>
       </c>
       <c r="F52" s="8" t="s">
-        <v>483</v>
+        <v>198</v>
       </c>
     </row>
     <row r="53" spans="1:6">
@@ -11832,16 +12789,16 @@
       </c>
       <c r="B53" s="12"/>
       <c r="C53" s="1" t="s">
-        <v>486</v>
+        <v>742</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>487</v>
+        <v>890</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>488</v>
+        <v>899</v>
       </c>
       <c r="F53" s="8" t="s">
-        <v>489</v>
+        <v>907</v>
       </c>
     </row>
     <row r="54" spans="1:6">
@@ -11868,16 +12825,16 @@
       </c>
       <c r="B55" s="12"/>
       <c r="C55" s="1" t="s">
-        <v>490</v>
+        <v>881</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>491</v>
+        <v>891</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>492</v>
+        <v>900</v>
       </c>
       <c r="F55" s="8" t="s">
-        <v>493</v>
+        <v>908</v>
       </c>
     </row>
     <row r="56" spans="1:6">
@@ -11886,16 +12843,16 @@
       </c>
       <c r="B56" s="12"/>
       <c r="C56" s="1" t="s">
-        <v>494</v>
+        <v>882</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>495</v>
+        <v>892</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>496</v>
+        <v>917</v>
       </c>
       <c r="F56" s="8" t="s">
-        <v>494</v>
+        <v>909</v>
       </c>
     </row>
     <row r="57" spans="1:6">
@@ -11904,16 +12861,16 @@
       </c>
       <c r="B57" s="12"/>
       <c r="C57" s="1" t="s">
-        <v>497</v>
+        <v>883</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>498</v>
+        <v>893</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>499</v>
+        <v>901</v>
       </c>
       <c r="F57" s="8" t="s">
-        <v>500</v>
+        <v>910</v>
       </c>
     </row>
     <row r="58" spans="1:6">
@@ -11940,16 +12897,16 @@
       </c>
       <c r="B59" s="12"/>
       <c r="C59" s="1" t="s">
-        <v>501</v>
+        <v>884</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>502</v>
+        <v>894</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>503</v>
+        <v>902</v>
       </c>
       <c r="F59" s="8" t="s">
-        <v>504</v>
+        <v>911</v>
       </c>
     </row>
     <row r="60" spans="1:6">
@@ -11958,16 +12915,16 @@
       </c>
       <c r="B60" s="12"/>
       <c r="C60" s="1" t="s">
-        <v>505</v>
+        <v>885</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>506</v>
+        <v>895</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>507</v>
+        <v>903</v>
       </c>
       <c r="F60" s="8" t="s">
-        <v>508</v>
+        <v>912</v>
       </c>
     </row>
     <row r="61" spans="1:6">
@@ -11978,16 +12935,16 @@
         <v>115</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>509</v>
+        <v>886</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>510</v>
+        <v>896</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>511</v>
+        <v>904</v>
       </c>
       <c r="F61" s="8" t="s">
-        <v>512</v>
+        <v>913</v>
       </c>
     </row>
     <row r="62" spans="1:6">
@@ -11996,16 +12953,16 @@
       </c>
       <c r="B62" s="12"/>
       <c r="C62" s="1" t="s">
-        <v>513</v>
+        <v>887</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>514</v>
+        <v>897</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>515</v>
+        <v>905</v>
       </c>
       <c r="F62" s="8" t="s">
-        <v>516</v>
+        <v>914</v>
       </c>
     </row>
     <row r="63" spans="1:6">
@@ -12014,16 +12971,16 @@
       </c>
       <c r="B63" s="12"/>
       <c r="C63" s="1" t="s">
-        <v>517</v>
+        <v>888</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>518</v>
+        <v>898</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>519</v>
+        <v>906</v>
       </c>
       <c r="F63" s="8" t="s">
-        <v>520</v>
+        <v>915</v>
       </c>
     </row>
     <row r="64" spans="1:6">
@@ -12032,16 +12989,16 @@
       </c>
       <c r="B64" s="12"/>
       <c r="C64" s="1" t="s">
-        <v>521</v>
+        <v>889</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>522</v>
+        <v>469</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>523</v>
+        <v>785</v>
       </c>
       <c r="F64" s="8" t="s">
-        <v>524</v>
+        <v>916</v>
       </c>
     </row>
     <row r="65" spans="1:6">
@@ -12115,6 +13072,7 @@
     <hyperlink ref="B34" r:id="rId2" location="'A3 500 - 100 GSM pack'!A1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -12122,8 +13080,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F68"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="F39" sqref="B39:F40"/>
+    <sheetView topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="C52" sqref="C52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -12135,14 +13093,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="43" t="s">
         <v>546</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="2" t="s">
@@ -12295,7 +13253,7 @@
         <v>17</v>
       </c>
       <c r="B16" s="32" t="s">
-        <v>527</v>
+        <v>918</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
@@ -12307,7 +13265,7 @@
         <v>19</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>525</v>
+        <v>919</v>
       </c>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
@@ -12407,21 +13365,21 @@
       <c r="F26" s="1"/>
     </row>
     <row r="29" spans="1:6">
-      <c r="A29" s="39" t="s">
+      <c r="A29" s="40" t="s">
         <v>475</v>
       </c>
-      <c r="B29" s="40"/>
-      <c r="C29" s="40"/>
-      <c r="D29" s="40"/>
-      <c r="E29" s="40"/>
-      <c r="F29" s="41"/>
+      <c r="B29" s="41"/>
+      <c r="C29" s="41"/>
+      <c r="D29" s="41"/>
+      <c r="E29" s="41"/>
+      <c r="F29" s="42"/>
     </row>
     <row r="30" spans="1:6">
       <c r="A30" s="7" t="s">
         <v>32</v>
       </c>
       <c r="B30" s="32" t="s">
-        <v>527</v>
+        <v>918</v>
       </c>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
@@ -12436,13 +13394,13 @@
         <v>34</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>477</v>
+        <v>920</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>36</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>478</v>
+        <v>594</v>
       </c>
       <c r="F31" s="8"/>
     </row>
@@ -12452,13 +13410,13 @@
         <v>38</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>479</v>
+        <v>595</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>40</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>480</v>
+        <v>596</v>
       </c>
       <c r="F32" s="8"/>
     </row>
@@ -12517,7 +13475,7 @@
         <v>51</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>52</v>
+        <v>244</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>53</v>
@@ -12714,16 +13672,16 @@
       </c>
       <c r="B52" s="12"/>
       <c r="C52" s="1" t="s">
-        <v>483</v>
+        <v>198</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>484</v>
+        <v>198</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>485</v>
-      </c>
-      <c r="F52" s="8" t="s">
-        <v>483</v>
+        <v>198</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>198</v>
       </c>
     </row>
     <row r="53" spans="1:6">
@@ -12732,16 +13690,16 @@
       </c>
       <c r="B53" s="12"/>
       <c r="C53" s="1" t="s">
-        <v>486</v>
+        <v>921</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>487</v>
+        <v>922</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>488</v>
+        <v>923</v>
       </c>
       <c r="F53" s="8" t="s">
-        <v>489</v>
+        <v>924</v>
       </c>
     </row>
     <row r="54" spans="1:6">
@@ -12768,16 +13726,16 @@
       </c>
       <c r="B55" s="12"/>
       <c r="C55" s="1" t="s">
-        <v>490</v>
+        <v>925</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>491</v>
+        <v>933</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>492</v>
+        <v>941</v>
       </c>
       <c r="F55" s="8" t="s">
-        <v>493</v>
+        <v>947</v>
       </c>
     </row>
     <row r="56" spans="1:6">
@@ -12786,16 +13744,16 @@
       </c>
       <c r="B56" s="12"/>
       <c r="C56" s="1" t="s">
-        <v>494</v>
+        <v>663</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>495</v>
+        <v>614</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>496</v>
+        <v>951</v>
       </c>
       <c r="F56" s="8" t="s">
-        <v>494</v>
+        <v>614</v>
       </c>
     </row>
     <row r="57" spans="1:6">
@@ -12804,16 +13762,16 @@
       </c>
       <c r="B57" s="12"/>
       <c r="C57" s="1" t="s">
-        <v>497</v>
+        <v>926</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>498</v>
+        <v>934</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>499</v>
+        <v>942</v>
       </c>
       <c r="F57" s="8" t="s">
-        <v>500</v>
+        <v>948</v>
       </c>
     </row>
     <row r="58" spans="1:6">
@@ -12840,16 +13798,16 @@
       </c>
       <c r="B59" s="12"/>
       <c r="C59" s="1" t="s">
-        <v>501</v>
+        <v>927</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>502</v>
+        <v>935</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>503</v>
+        <v>943</v>
       </c>
       <c r="F59" s="8" t="s">
-        <v>504</v>
+        <v>616</v>
       </c>
     </row>
     <row r="60" spans="1:6">
@@ -12858,16 +13816,16 @@
       </c>
       <c r="B60" s="12"/>
       <c r="C60" s="1" t="s">
-        <v>505</v>
+        <v>928</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>506</v>
+        <v>936</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>507</v>
+        <v>944</v>
       </c>
       <c r="F60" s="8" t="s">
-        <v>508</v>
+        <v>949</v>
       </c>
     </row>
     <row r="61" spans="1:6">
@@ -12878,16 +13836,16 @@
         <v>115</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>509</v>
+        <v>929</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>510</v>
+        <v>937</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>511</v>
+        <v>945</v>
       </c>
       <c r="F61" s="8" t="s">
-        <v>512</v>
+        <v>631</v>
       </c>
     </row>
     <row r="62" spans="1:6">
@@ -12896,16 +13854,16 @@
       </c>
       <c r="B62" s="12"/>
       <c r="C62" s="1" t="s">
-        <v>513</v>
+        <v>930</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>514</v>
+        <v>938</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>515</v>
+        <v>946</v>
       </c>
       <c r="F62" s="8" t="s">
-        <v>516</v>
+        <v>950</v>
       </c>
     </row>
     <row r="63" spans="1:6">
@@ -12914,16 +13872,16 @@
       </c>
       <c r="B63" s="12"/>
       <c r="C63" s="1" t="s">
-        <v>517</v>
+        <v>931</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>518</v>
+        <v>939</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>519</v>
+        <v>266</v>
       </c>
       <c r="F63" s="8" t="s">
-        <v>520</v>
+        <v>633</v>
       </c>
     </row>
     <row r="64" spans="1:6">
@@ -12932,16 +13890,16 @@
       </c>
       <c r="B64" s="12"/>
       <c r="C64" s="1" t="s">
-        <v>521</v>
+        <v>932</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>522</v>
+        <v>940</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>523</v>
+        <v>754</v>
       </c>
       <c r="F64" s="8" t="s">
-        <v>524</v>
+        <v>754</v>
       </c>
     </row>
     <row r="65" spans="1:6">
@@ -13036,14 +13994,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="39" t="s">
         <v>239</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="2" t="s">
@@ -13921,8 +14879,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F68"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="F39" sqref="B39:F40"/>
+    <sheetView topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="B65" sqref="B65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -13934,14 +14892,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="43" t="s">
         <v>547</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="2" t="s">
@@ -14094,7 +15052,7 @@
         <v>17</v>
       </c>
       <c r="B16" s="32" t="s">
-        <v>527</v>
+        <v>952</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
@@ -14206,21 +15164,21 @@
       <c r="F26" s="1"/>
     </row>
     <row r="29" spans="1:6">
-      <c r="A29" s="39" t="s">
+      <c r="A29" s="40" t="s">
         <v>475</v>
       </c>
-      <c r="B29" s="40"/>
-      <c r="C29" s="40"/>
-      <c r="D29" s="40"/>
-      <c r="E29" s="40"/>
-      <c r="F29" s="41"/>
+      <c r="B29" s="41"/>
+      <c r="C29" s="41"/>
+      <c r="D29" s="41"/>
+      <c r="E29" s="41"/>
+      <c r="F29" s="42"/>
     </row>
     <row r="30" spans="1:6">
       <c r="A30" s="7" t="s">
         <v>32</v>
       </c>
       <c r="B30" s="32" t="s">
-        <v>527</v>
+        <v>952</v>
       </c>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
@@ -14235,13 +15193,13 @@
         <v>34</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>477</v>
+        <v>953</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>36</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>478</v>
+        <v>954</v>
       </c>
       <c r="F31" s="8"/>
     </row>
@@ -14251,13 +15209,13 @@
         <v>38</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>479</v>
+        <v>955</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>40</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>480</v>
+        <v>956</v>
       </c>
       <c r="F32" s="8"/>
     </row>
@@ -14316,7 +15274,7 @@
         <v>51</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>52</v>
+        <v>244</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>53</v>
@@ -14513,16 +15471,16 @@
       </c>
       <c r="B52" s="12"/>
       <c r="C52" s="1" t="s">
-        <v>483</v>
+        <v>198</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>484</v>
+        <v>198</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>485</v>
+        <v>198</v>
       </c>
       <c r="F52" s="8" t="s">
-        <v>483</v>
+        <v>198</v>
       </c>
     </row>
     <row r="53" spans="1:6">
@@ -14531,16 +15489,16 @@
       </c>
       <c r="B53" s="12"/>
       <c r="C53" s="1" t="s">
-        <v>486</v>
+        <v>598</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>487</v>
+        <v>957</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>488</v>
+        <v>964</v>
       </c>
       <c r="F53" s="8" t="s">
-        <v>489</v>
+        <v>975</v>
       </c>
     </row>
     <row r="54" spans="1:6">
@@ -14567,16 +15525,16 @@
       </c>
       <c r="B55" s="12"/>
       <c r="C55" s="1" t="s">
-        <v>490</v>
+        <v>602</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>491</v>
+        <v>958</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>492</v>
+        <v>965</v>
       </c>
       <c r="F55" s="8" t="s">
-        <v>493</v>
+        <v>976</v>
       </c>
     </row>
     <row r="56" spans="1:6">
@@ -14585,16 +15543,16 @@
       </c>
       <c r="B56" s="12"/>
       <c r="C56" s="1" t="s">
-        <v>494</v>
+        <v>603</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>495</v>
+        <v>614</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>496</v>
+        <v>966</v>
       </c>
       <c r="F56" s="8" t="s">
-        <v>494</v>
+        <v>977</v>
       </c>
     </row>
     <row r="57" spans="1:6">
@@ -14603,16 +15561,16 @@
       </c>
       <c r="B57" s="12"/>
       <c r="C57" s="1" t="s">
-        <v>497</v>
+        <v>604</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>498</v>
+        <v>959</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>499</v>
+        <v>967</v>
       </c>
       <c r="F57" s="8" t="s">
-        <v>500</v>
+        <v>978</v>
       </c>
     </row>
     <row r="58" spans="1:6">
@@ -14639,16 +15597,16 @@
       </c>
       <c r="B59" s="12"/>
       <c r="C59" s="1" t="s">
-        <v>501</v>
+        <v>605</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>502</v>
+        <v>969</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>503</v>
+        <v>968</v>
       </c>
       <c r="F59" s="8" t="s">
-        <v>504</v>
+        <v>979</v>
       </c>
     </row>
     <row r="60" spans="1:6">
@@ -14657,16 +15615,16 @@
       </c>
       <c r="B60" s="12"/>
       <c r="C60" s="1" t="s">
-        <v>505</v>
+        <v>606</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>506</v>
+        <v>960</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>507</v>
+        <v>970</v>
       </c>
       <c r="F60" s="8" t="s">
-        <v>508</v>
+        <v>980</v>
       </c>
     </row>
     <row r="61" spans="1:6">
@@ -14677,16 +15635,16 @@
         <v>115</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>509</v>
+        <v>624</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>510</v>
+        <v>961</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>511</v>
+        <v>971</v>
       </c>
       <c r="F61" s="8" t="s">
-        <v>512</v>
+        <v>981</v>
       </c>
     </row>
     <row r="62" spans="1:6">
@@ -14695,16 +15653,16 @@
       </c>
       <c r="B62" s="12"/>
       <c r="C62" s="1" t="s">
-        <v>513</v>
+        <v>625</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>514</v>
+        <v>962</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>515</v>
+        <v>972</v>
       </c>
       <c r="F62" s="8" t="s">
-        <v>516</v>
+        <v>982</v>
       </c>
     </row>
     <row r="63" spans="1:6">
@@ -14713,16 +15671,16 @@
       </c>
       <c r="B63" s="12"/>
       <c r="C63" s="1" t="s">
-        <v>517</v>
+        <v>607</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>518</v>
+        <v>963</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>519</v>
+        <v>973</v>
       </c>
       <c r="F63" s="8" t="s">
-        <v>520</v>
+        <v>983</v>
       </c>
     </row>
     <row r="64" spans="1:6">
@@ -14731,16 +15689,16 @@
       </c>
       <c r="B64" s="12"/>
       <c r="C64" s="1" t="s">
-        <v>521</v>
+        <v>626</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>522</v>
+        <v>630</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>523</v>
+        <v>974</v>
       </c>
       <c r="F64" s="8" t="s">
-        <v>524</v>
+        <v>744</v>
       </c>
     </row>
     <row r="65" spans="1:6">
@@ -14814,6 +15772,7 @@
     <hyperlink ref="B34" r:id="rId2" location="'A3 500 - 200 GSM pack'!A1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -14821,8 +15780,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F68"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="F39" sqref="B39:F40"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -14834,14 +15793,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="43" t="s">
         <v>548</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="2" t="s">
@@ -14994,7 +15953,7 @@
         <v>17</v>
       </c>
       <c r="B16" s="32" t="s">
-        <v>527</v>
+        <v>1017</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
@@ -15006,7 +15965,7 @@
         <v>19</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>525</v>
+        <v>1018</v>
       </c>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
@@ -15106,21 +16065,21 @@
       <c r="F26" s="1"/>
     </row>
     <row r="29" spans="1:6">
-      <c r="A29" s="39" t="s">
+      <c r="A29" s="40" t="s">
         <v>475</v>
       </c>
-      <c r="B29" s="40"/>
-      <c r="C29" s="40"/>
-      <c r="D29" s="40"/>
-      <c r="E29" s="40"/>
-      <c r="F29" s="41"/>
+      <c r="B29" s="41"/>
+      <c r="C29" s="41"/>
+      <c r="D29" s="41"/>
+      <c r="E29" s="41"/>
+      <c r="F29" s="42"/>
     </row>
     <row r="30" spans="1:6">
       <c r="A30" s="7" t="s">
         <v>32</v>
       </c>
       <c r="B30" s="32" t="s">
-        <v>527</v>
+        <v>1017</v>
       </c>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
@@ -15135,13 +16094,13 @@
         <v>34</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>477</v>
+        <v>595</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>36</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>478</v>
+        <v>594</v>
       </c>
       <c r="F31" s="8"/>
     </row>
@@ -15151,13 +16110,13 @@
         <v>38</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>479</v>
+        <v>984</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>40</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>480</v>
+        <v>985</v>
       </c>
       <c r="F32" s="8"/>
     </row>
@@ -15177,7 +16136,7 @@
       <c r="A34" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="B34" s="35" t="s">
+      <c r="B34" s="38" t="s">
         <v>534</v>
       </c>
       <c r="C34" s="3" t="s">
@@ -15216,7 +16175,7 @@
         <v>51</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>52</v>
+        <v>244</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>53</v>
@@ -15413,16 +16372,16 @@
       </c>
       <c r="B52" s="12"/>
       <c r="C52" s="1" t="s">
-        <v>483</v>
+        <v>198</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>484</v>
+        <v>198</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>485</v>
+        <v>198</v>
       </c>
       <c r="F52" s="8" t="s">
-        <v>483</v>
+        <v>198</v>
       </c>
     </row>
     <row r="53" spans="1:6">
@@ -15431,16 +16390,16 @@
       </c>
       <c r="B53" s="12"/>
       <c r="C53" s="1" t="s">
-        <v>486</v>
+        <v>986</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>487</v>
+        <v>995</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>488</v>
+        <v>1001</v>
       </c>
       <c r="F53" s="8" t="s">
-        <v>489</v>
+        <v>1009</v>
       </c>
     </row>
     <row r="54" spans="1:6">
@@ -15467,16 +16426,16 @@
       </c>
       <c r="B55" s="12"/>
       <c r="C55" s="1" t="s">
-        <v>490</v>
+        <v>987</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>491</v>
+        <v>996</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>492</v>
+        <v>1002</v>
       </c>
       <c r="F55" s="8" t="s">
-        <v>493</v>
+        <v>1010</v>
       </c>
     </row>
     <row r="56" spans="1:6">
@@ -15485,16 +16444,16 @@
       </c>
       <c r="B56" s="12"/>
       <c r="C56" s="1" t="s">
-        <v>494</v>
+        <v>988</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>495</v>
+        <v>966</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>496</v>
+        <v>748</v>
       </c>
       <c r="F56" s="8" t="s">
-        <v>494</v>
+        <v>822</v>
       </c>
     </row>
     <row r="57" spans="1:6">
@@ -15503,16 +16462,16 @@
       </c>
       <c r="B57" s="12"/>
       <c r="C57" s="1" t="s">
-        <v>497</v>
+        <v>989</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>498</v>
+        <v>976</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>499</v>
+        <v>1003</v>
       </c>
       <c r="F57" s="8" t="s">
-        <v>500</v>
+        <v>1011</v>
       </c>
     </row>
     <row r="58" spans="1:6">
@@ -15539,16 +16498,16 @@
       </c>
       <c r="B59" s="12"/>
       <c r="C59" s="1" t="s">
-        <v>501</v>
+        <v>990</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>502</v>
+        <v>997</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>503</v>
+        <v>1004</v>
       </c>
       <c r="F59" s="8" t="s">
-        <v>504</v>
+        <v>1012</v>
       </c>
     </row>
     <row r="60" spans="1:6">
@@ -15557,16 +16516,16 @@
       </c>
       <c r="B60" s="12"/>
       <c r="C60" s="1" t="s">
-        <v>505</v>
+        <v>991</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>506</v>
+        <v>998</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>507</v>
+        <v>1005</v>
       </c>
       <c r="F60" s="8" t="s">
-        <v>508</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="61" spans="1:6">
@@ -15577,16 +16536,16 @@
         <v>115</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>509</v>
+        <v>992</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>510</v>
+        <v>999</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>511</v>
+        <v>1006</v>
       </c>
       <c r="F61" s="8" t="s">
-        <v>512</v>
+        <v>1014</v>
       </c>
     </row>
     <row r="62" spans="1:6">
@@ -15595,16 +16554,16 @@
       </c>
       <c r="B62" s="12"/>
       <c r="C62" s="1" t="s">
-        <v>513</v>
+        <v>993</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>514</v>
+        <v>1000</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>515</v>
+        <v>1007</v>
       </c>
       <c r="F62" s="8" t="s">
-        <v>516</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="63" spans="1:6">
@@ -15613,16 +16572,16 @@
       </c>
       <c r="B63" s="12"/>
       <c r="C63" s="1" t="s">
-        <v>517</v>
+        <v>994</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>518</v>
+        <v>311</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>519</v>
+        <v>1008</v>
       </c>
       <c r="F63" s="8" t="s">
-        <v>520</v>
+        <v>1016</v>
       </c>
     </row>
     <row r="64" spans="1:6">
@@ -15631,16 +16590,16 @@
       </c>
       <c r="B64" s="12"/>
       <c r="C64" s="1" t="s">
-        <v>521</v>
+        <v>744</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>522</v>
+        <v>376</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>523</v>
+        <v>618</v>
       </c>
       <c r="F64" s="8" t="s">
-        <v>524</v>
+        <v>932</v>
       </c>
     </row>
     <row r="65" spans="1:6">
@@ -15714,6 +16673,7 @@
     <hyperlink ref="B34" r:id="rId2" location="'A3 500 - 250 GSM pack'!A1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -15721,8 +16681,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F68"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="F39" sqref="B39:F40"/>
+    <sheetView topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="F73" sqref="F73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -15734,14 +16694,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="43" t="s">
         <v>549</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="2" t="s">
@@ -15894,7 +16854,7 @@
         <v>17</v>
       </c>
       <c r="B16" s="32" t="s">
-        <v>527</v>
+        <v>1022</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
@@ -15906,7 +16866,7 @@
         <v>19</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>525</v>
+        <v>1023</v>
       </c>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
@@ -16006,21 +16966,21 @@
       <c r="F26" s="1"/>
     </row>
     <row r="29" spans="1:6">
-      <c r="A29" s="39" t="s">
+      <c r="A29" s="40" t="s">
         <v>475</v>
       </c>
-      <c r="B29" s="40"/>
-      <c r="C29" s="40"/>
-      <c r="D29" s="40"/>
-      <c r="E29" s="40"/>
-      <c r="F29" s="41"/>
+      <c r="B29" s="41"/>
+      <c r="C29" s="41"/>
+      <c r="D29" s="41"/>
+      <c r="E29" s="41"/>
+      <c r="F29" s="42"/>
     </row>
     <row r="30" spans="1:6">
       <c r="A30" s="7" t="s">
         <v>32</v>
       </c>
       <c r="B30" s="32" t="s">
-        <v>527</v>
+        <v>1022</v>
       </c>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
@@ -16035,13 +16995,13 @@
         <v>34</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>477</v>
+        <v>1019</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>36</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>478</v>
+        <v>636</v>
       </c>
       <c r="F31" s="8"/>
     </row>
@@ -16051,13 +17011,13 @@
         <v>38</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>479</v>
+        <v>1020</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>40</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>480</v>
+        <v>1021</v>
       </c>
       <c r="F32" s="8"/>
     </row>
@@ -16116,7 +17076,7 @@
         <v>51</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>52</v>
+        <v>244</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>53</v>
@@ -16313,16 +17273,16 @@
       </c>
       <c r="B52" s="12"/>
       <c r="C52" s="1" t="s">
-        <v>483</v>
+        <v>198</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>484</v>
+        <v>198</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>485</v>
-      </c>
-      <c r="F52" s="8" t="s">
-        <v>483</v>
+        <v>198</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>198</v>
       </c>
     </row>
     <row r="53" spans="1:6">
@@ -16331,16 +17291,16 @@
       </c>
       <c r="B53" s="12"/>
       <c r="C53" s="1" t="s">
-        <v>486</v>
+        <v>1024</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>487</v>
+        <v>1029</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>488</v>
+        <v>1034</v>
       </c>
       <c r="F53" s="8" t="s">
-        <v>489</v>
+        <v>601</v>
       </c>
     </row>
     <row r="54" spans="1:6">
@@ -16367,16 +17327,16 @@
       </c>
       <c r="B55" s="12"/>
       <c r="C55" s="1" t="s">
-        <v>490</v>
+        <v>1025</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>491</v>
+        <v>1030</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>492</v>
+        <v>1035</v>
       </c>
       <c r="F55" s="8" t="s">
-        <v>493</v>
+        <v>619</v>
       </c>
     </row>
     <row r="56" spans="1:6">
@@ -16385,16 +17345,16 @@
       </c>
       <c r="B56" s="12"/>
       <c r="C56" s="1" t="s">
-        <v>494</v>
+        <v>809</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>495</v>
+        <v>809</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>496</v>
+        <v>1036</v>
       </c>
       <c r="F56" s="8" t="s">
-        <v>494</v>
+        <v>577</v>
       </c>
     </row>
     <row r="57" spans="1:6">
@@ -16403,16 +17363,16 @@
       </c>
       <c r="B57" s="12"/>
       <c r="C57" s="1" t="s">
-        <v>497</v>
+        <v>1026</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>498</v>
+        <v>1031</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>499</v>
+        <v>1037</v>
       </c>
       <c r="F57" s="8" t="s">
-        <v>500</v>
+        <v>620</v>
       </c>
     </row>
     <row r="58" spans="1:6">
@@ -16439,16 +17399,16 @@
       </c>
       <c r="B59" s="12"/>
       <c r="C59" s="1" t="s">
-        <v>501</v>
+        <v>811</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>502</v>
+        <v>1032</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>503</v>
+        <v>1038</v>
       </c>
       <c r="F59" s="8" t="s">
-        <v>504</v>
+        <v>623</v>
       </c>
     </row>
     <row r="60" spans="1:6">
@@ -16457,16 +17417,16 @@
       </c>
       <c r="B60" s="12"/>
       <c r="C60" s="1" t="s">
-        <v>505</v>
+        <v>1027</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>506</v>
+        <v>1033</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>507</v>
+        <v>1039</v>
       </c>
       <c r="F60" s="8" t="s">
-        <v>508</v>
+        <v>621</v>
       </c>
     </row>
     <row r="61" spans="1:6">
@@ -16477,16 +17437,16 @@
         <v>115</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>509</v>
+        <v>1041</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>510</v>
+        <v>1043</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>511</v>
+        <v>1045</v>
       </c>
       <c r="F61" s="8" t="s">
-        <v>512</v>
+        <v>634</v>
       </c>
     </row>
     <row r="62" spans="1:6">
@@ -16495,16 +17455,16 @@
       </c>
       <c r="B62" s="12"/>
       <c r="C62" s="1" t="s">
-        <v>513</v>
+        <v>1042</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>514</v>
+        <v>1044</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>515</v>
+        <v>1046</v>
       </c>
       <c r="F62" s="8" t="s">
-        <v>516</v>
+        <v>635</v>
       </c>
     </row>
     <row r="63" spans="1:6">
@@ -16513,16 +17473,16 @@
       </c>
       <c r="B63" s="12"/>
       <c r="C63" s="1" t="s">
-        <v>517</v>
+        <v>834</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>518</v>
+        <v>697</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>519</v>
+        <v>1040</v>
       </c>
       <c r="F63" s="8" t="s">
-        <v>520</v>
+        <v>622</v>
       </c>
     </row>
     <row r="64" spans="1:6">
@@ -16531,16 +17491,16 @@
       </c>
       <c r="B64" s="12"/>
       <c r="C64" s="1" t="s">
-        <v>521</v>
+        <v>1028</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>522</v>
+        <v>1028</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>523</v>
+        <v>376</v>
       </c>
       <c r="F64" s="8" t="s">
-        <v>524</v>
+        <v>374</v>
       </c>
     </row>
     <row r="65" spans="1:6">
@@ -16622,8 +17582,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F68"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="F39" sqref="B39:F40"/>
+    <sheetView topLeftCell="D46" workbookViewId="0">
+      <selection activeCell="F66" sqref="F66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -16635,14 +17595,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="43" t="s">
         <v>550</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="2" t="s">
@@ -16795,7 +17755,7 @@
         <v>17</v>
       </c>
       <c r="B16" s="32" t="s">
-        <v>527</v>
+        <v>1047</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
@@ -16807,7 +17767,7 @@
         <v>19</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>525</v>
+        <v>1048</v>
       </c>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
@@ -16907,21 +17867,21 @@
       <c r="F26" s="1"/>
     </row>
     <row r="29" spans="1:6">
-      <c r="A29" s="39" t="s">
+      <c r="A29" s="40" t="s">
         <v>475</v>
       </c>
-      <c r="B29" s="40"/>
-      <c r="C29" s="40"/>
-      <c r="D29" s="40"/>
-      <c r="E29" s="40"/>
-      <c r="F29" s="41"/>
+      <c r="B29" s="41"/>
+      <c r="C29" s="41"/>
+      <c r="D29" s="41"/>
+      <c r="E29" s="41"/>
+      <c r="F29" s="42"/>
     </row>
     <row r="30" spans="1:6">
       <c r="A30" s="7" t="s">
         <v>32</v>
       </c>
       <c r="B30" s="32" t="s">
-        <v>527</v>
+        <v>1047</v>
       </c>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
@@ -16936,13 +17896,13 @@
         <v>34</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>477</v>
+        <v>596</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>36</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>478</v>
+        <v>1049</v>
       </c>
       <c r="F31" s="8"/>
     </row>
@@ -16952,13 +17912,13 @@
         <v>38</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>479</v>
+        <v>1050</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>40</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>480</v>
+        <v>1051</v>
       </c>
       <c r="F32" s="8"/>
     </row>
@@ -17214,16 +18174,16 @@
       </c>
       <c r="B52" s="12"/>
       <c r="C52" s="1" t="s">
-        <v>483</v>
+        <v>198</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>484</v>
+        <v>198</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>485</v>
+        <v>198</v>
       </c>
       <c r="F52" s="8" t="s">
-        <v>483</v>
+        <v>198</v>
       </c>
     </row>
     <row r="53" spans="1:6">
@@ -17232,16 +18192,16 @@
       </c>
       <c r="B53" s="12"/>
       <c r="C53" s="1" t="s">
-        <v>486</v>
+        <v>1052</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>487</v>
+        <v>1060</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>488</v>
+        <v>1068</v>
       </c>
       <c r="F53" s="8" t="s">
-        <v>489</v>
+        <v>1077</v>
       </c>
     </row>
     <row r="54" spans="1:6">
@@ -17268,16 +18228,16 @@
       </c>
       <c r="B55" s="12"/>
       <c r="C55" s="1" t="s">
-        <v>490</v>
+        <v>1053</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>491</v>
+        <v>1061</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>492</v>
+        <v>1069</v>
       </c>
       <c r="F55" s="8" t="s">
-        <v>493</v>
+        <v>1078</v>
       </c>
     </row>
     <row r="56" spans="1:6">
@@ -17286,16 +18246,16 @@
       </c>
       <c r="B56" s="12"/>
       <c r="C56" s="1" t="s">
-        <v>494</v>
+        <v>737</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>495</v>
+        <v>822</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>496</v>
+        <v>966</v>
       </c>
       <c r="F56" s="8" t="s">
-        <v>494</v>
+        <v>577</v>
       </c>
     </row>
     <row r="57" spans="1:6">
@@ -17304,16 +18264,16 @@
       </c>
       <c r="B57" s="12"/>
       <c r="C57" s="1" t="s">
-        <v>497</v>
+        <v>1054</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>498</v>
+        <v>1062</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>499</v>
+        <v>1070</v>
       </c>
       <c r="F57" s="8" t="s">
-        <v>500</v>
+        <v>1079</v>
       </c>
     </row>
     <row r="58" spans="1:6">
@@ -17340,16 +18300,16 @@
       </c>
       <c r="B59" s="12"/>
       <c r="C59" s="1" t="s">
-        <v>501</v>
+        <v>1055</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>502</v>
+        <v>1063</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>503</v>
+        <v>1071</v>
       </c>
       <c r="F59" s="8" t="s">
-        <v>504</v>
+        <v>730</v>
       </c>
     </row>
     <row r="60" spans="1:6">
@@ -17358,16 +18318,16 @@
       </c>
       <c r="B60" s="12"/>
       <c r="C60" s="1" t="s">
-        <v>505</v>
+        <v>1056</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>506</v>
+        <v>1064</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>507</v>
+        <v>1072</v>
       </c>
       <c r="F60" s="8" t="s">
-        <v>508</v>
+        <v>1080</v>
       </c>
     </row>
     <row r="61" spans="1:6">
@@ -17378,16 +18338,16 @@
         <v>115</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>509</v>
+        <v>1057</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>510</v>
+        <v>1065</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>511</v>
+        <v>1073</v>
       </c>
       <c r="F61" s="8" t="s">
-        <v>512</v>
+        <v>581</v>
       </c>
     </row>
     <row r="62" spans="1:6">
@@ -17396,16 +18356,16 @@
       </c>
       <c r="B62" s="12"/>
       <c r="C62" s="1" t="s">
-        <v>513</v>
+        <v>1058</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>514</v>
+        <v>1066</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>515</v>
+        <v>1074</v>
       </c>
       <c r="F62" s="8" t="s">
-        <v>516</v>
+        <v>1081</v>
       </c>
     </row>
     <row r="63" spans="1:6">
@@ -17414,16 +18374,16 @@
       </c>
       <c r="B63" s="12"/>
       <c r="C63" s="1" t="s">
-        <v>517</v>
+        <v>1059</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>518</v>
+        <v>1067</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>519</v>
+        <v>1075</v>
       </c>
       <c r="F63" s="8" t="s">
-        <v>520</v>
+        <v>732</v>
       </c>
     </row>
     <row r="64" spans="1:6">
@@ -17432,16 +18392,16 @@
       </c>
       <c r="B64" s="12"/>
       <c r="C64" s="1" t="s">
-        <v>521</v>
+        <v>744</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>522</v>
+        <v>932</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>523</v>
+        <v>1076</v>
       </c>
       <c r="F64" s="8" t="s">
-        <v>524</v>
+        <v>679</v>
       </c>
     </row>
     <row r="65" spans="1:6">
@@ -17515,6 +18475,7 @@
     <hyperlink ref="B34" r:id="rId2" location="'A3 500 - 350 GSM pack'!A1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -17522,8 +18483,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F68"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="F39" sqref="B39:F40"/>
+    <sheetView topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="F64" sqref="F64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -17535,14 +18496,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="43" t="s">
         <v>546</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="2" t="s">
@@ -17695,7 +18656,7 @@
         <v>17</v>
       </c>
       <c r="B16" s="32" t="s">
-        <v>527</v>
+        <v>1082</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
@@ -17707,7 +18668,7 @@
         <v>19</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>525</v>
+        <v>1083</v>
       </c>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
@@ -17807,21 +18768,21 @@
       <c r="F26" s="1"/>
     </row>
     <row r="29" spans="1:6">
-      <c r="A29" s="39" t="s">
+      <c r="A29" s="40" t="s">
         <v>475</v>
       </c>
-      <c r="B29" s="40"/>
-      <c r="C29" s="40"/>
-      <c r="D29" s="40"/>
-      <c r="E29" s="40"/>
-      <c r="F29" s="41"/>
+      <c r="B29" s="41"/>
+      <c r="C29" s="41"/>
+      <c r="D29" s="41"/>
+      <c r="E29" s="41"/>
+      <c r="F29" s="42"/>
     </row>
     <row r="30" spans="1:6">
       <c r="A30" s="7" t="s">
         <v>32</v>
       </c>
       <c r="B30" s="32" t="s">
-        <v>527</v>
+        <v>1082</v>
       </c>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
@@ -17836,13 +18797,13 @@
         <v>34</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>477</v>
+        <v>1084</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>36</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>478</v>
+        <v>637</v>
       </c>
       <c r="F31" s="8"/>
     </row>
@@ -17852,13 +18813,13 @@
         <v>38</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>479</v>
+        <v>985</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>40</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>480</v>
+        <v>1085</v>
       </c>
       <c r="F32" s="8"/>
     </row>
@@ -17917,13 +18878,13 @@
         <v>51</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>52</v>
+        <v>244</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>53</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="E37" s="1"/>
       <c r="F37" s="8"/>
@@ -18114,16 +19075,16 @@
       </c>
       <c r="B52" s="12"/>
       <c r="C52" s="1" t="s">
-        <v>483</v>
+        <v>198</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>484</v>
+        <v>198</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>485</v>
-      </c>
-      <c r="F52" s="8" t="s">
-        <v>483</v>
+        <v>198</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>198</v>
       </c>
     </row>
     <row r="53" spans="1:6">
@@ -18132,16 +19093,16 @@
       </c>
       <c r="B53" s="12"/>
       <c r="C53" s="1" t="s">
-        <v>486</v>
+        <v>1086</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>487</v>
+        <v>1095</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>488</v>
+        <v>1104</v>
       </c>
       <c r="F53" s="8" t="s">
-        <v>489</v>
+        <v>1110</v>
       </c>
     </row>
     <row r="54" spans="1:6">
@@ -18168,16 +19129,16 @@
       </c>
       <c r="B55" s="12"/>
       <c r="C55" s="1" t="s">
-        <v>490</v>
+        <v>1087</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>491</v>
+        <v>1096</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>492</v>
+        <v>615</v>
       </c>
       <c r="F55" s="8" t="s">
-        <v>493</v>
+        <v>1111</v>
       </c>
     </row>
     <row r="56" spans="1:6">
@@ -18186,16 +19147,16 @@
       </c>
       <c r="B56" s="12"/>
       <c r="C56" s="1" t="s">
-        <v>494</v>
+        <v>557</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>495</v>
+        <v>815</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>496</v>
+        <v>951</v>
       </c>
       <c r="F56" s="8" t="s">
-        <v>494</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="57" spans="1:6">
@@ -18204,16 +19165,16 @@
       </c>
       <c r="B57" s="12"/>
       <c r="C57" s="1" t="s">
-        <v>497</v>
+        <v>1088</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>498</v>
+        <v>1097</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>499</v>
+        <v>1105</v>
       </c>
       <c r="F57" s="8" t="s">
-        <v>500</v>
+        <v>1113</v>
       </c>
     </row>
     <row r="58" spans="1:6">
@@ -18240,16 +19201,16 @@
       </c>
       <c r="B59" s="12"/>
       <c r="C59" s="1" t="s">
-        <v>501</v>
+        <v>1089</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>502</v>
+        <v>1098</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>503</v>
+        <v>1106</v>
       </c>
       <c r="F59" s="8" t="s">
-        <v>504</v>
+        <v>1114</v>
       </c>
     </row>
     <row r="60" spans="1:6">
@@ -18258,16 +19219,16 @@
       </c>
       <c r="B60" s="12"/>
       <c r="C60" s="1" t="s">
-        <v>505</v>
+        <v>1090</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>506</v>
+        <v>1099</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>507</v>
+        <v>1107</v>
       </c>
       <c r="F60" s="8" t="s">
-        <v>508</v>
+        <v>1115</v>
       </c>
     </row>
     <row r="61" spans="1:6">
@@ -18278,16 +19239,16 @@
         <v>115</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>509</v>
+        <v>1091</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>510</v>
+        <v>1100</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>511</v>
+        <v>1108</v>
       </c>
       <c r="F61" s="8" t="s">
-        <v>512</v>
+        <v>1116</v>
       </c>
     </row>
     <row r="62" spans="1:6">
@@ -18296,16 +19257,16 @@
       </c>
       <c r="B62" s="12"/>
       <c r="C62" s="1" t="s">
-        <v>513</v>
+        <v>1092</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>514</v>
+        <v>1101</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>515</v>
+        <v>1119</v>
       </c>
       <c r="F62" s="8" t="s">
-        <v>516</v>
+        <v>1117</v>
       </c>
     </row>
     <row r="63" spans="1:6">
@@ -18314,16 +19275,16 @@
       </c>
       <c r="B63" s="12"/>
       <c r="C63" s="1" t="s">
-        <v>517</v>
+        <v>1093</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>518</v>
+        <v>1102</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>519</v>
+        <v>1109</v>
       </c>
       <c r="F63" s="8" t="s">
-        <v>520</v>
+        <v>1118</v>
       </c>
     </row>
     <row r="64" spans="1:6">
@@ -18332,16 +19293,16 @@
       </c>
       <c r="B64" s="12"/>
       <c r="C64" s="1" t="s">
-        <v>521</v>
+        <v>1094</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>522</v>
+        <v>1103</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>523</v>
+        <v>618</v>
       </c>
       <c r="F64" s="8" t="s">
-        <v>524</v>
+        <v>795</v>
       </c>
     </row>
     <row r="65" spans="1:6">
@@ -18422,8 +19383,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F68"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" topLeftCell="D46" workbookViewId="0">
+      <selection activeCell="E54" sqref="E54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -18435,14 +19396,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="43" t="s">
         <v>546</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="2" t="s">
@@ -18595,7 +19556,7 @@
         <v>17</v>
       </c>
       <c r="B16" s="32" t="s">
-        <v>527</v>
+        <v>1120</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
@@ -18607,7 +19568,7 @@
         <v>19</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>525</v>
+        <v>1121</v>
       </c>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
@@ -18707,21 +19668,21 @@
       <c r="F26" s="1"/>
     </row>
     <row r="29" spans="1:6">
-      <c r="A29" s="39" t="s">
+      <c r="A29" s="40" t="s">
         <v>475</v>
       </c>
-      <c r="B29" s="40"/>
-      <c r="C29" s="40"/>
-      <c r="D29" s="40"/>
-      <c r="E29" s="40"/>
-      <c r="F29" s="41"/>
+      <c r="B29" s="41"/>
+      <c r="C29" s="41"/>
+      <c r="D29" s="41"/>
+      <c r="E29" s="41"/>
+      <c r="F29" s="42"/>
     </row>
     <row r="30" spans="1:6">
       <c r="A30" s="7" t="s">
         <v>32</v>
       </c>
       <c r="B30" s="32" t="s">
-        <v>527</v>
+        <v>1120</v>
       </c>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
@@ -18823,7 +19784,7 @@
         <v>53</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="E37" s="1"/>
       <c r="F37" s="8"/>
@@ -18833,7 +19794,7 @@
         <v>55</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>52</v>
+        <v>244</v>
       </c>
       <c r="C38" s="1"/>
       <c r="D38" s="1"/>
@@ -19014,16 +19975,16 @@
       </c>
       <c r="B52" s="12"/>
       <c r="C52" s="1" t="s">
-        <v>483</v>
+        <v>198</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>484</v>
+        <v>198</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>485</v>
+        <v>198</v>
       </c>
       <c r="F52" s="8" t="s">
-        <v>483</v>
+        <v>198</v>
       </c>
     </row>
     <row r="53" spans="1:6">
@@ -19032,16 +19993,16 @@
       </c>
       <c r="B53" s="12"/>
       <c r="C53" s="1" t="s">
-        <v>486</v>
+        <v>1122</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>487</v>
+        <v>1132</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>488</v>
+        <v>1141</v>
       </c>
       <c r="F53" s="8" t="s">
-        <v>489</v>
+        <v>1151</v>
       </c>
     </row>
     <row r="54" spans="1:6">
@@ -19050,16 +20011,16 @@
       </c>
       <c r="B54" s="12"/>
       <c r="C54" s="1" t="s">
-        <v>153</v>
+        <v>702</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>153</v>
+        <v>702</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>153</v>
+        <v>713</v>
       </c>
       <c r="F54" s="8" t="s">
-        <v>153</v>
+        <v>702</v>
       </c>
     </row>
     <row r="55" spans="1:6">
@@ -19068,16 +20029,16 @@
       </c>
       <c r="B55" s="12"/>
       <c r="C55" s="1" t="s">
-        <v>490</v>
+        <v>1123</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>491</v>
+        <v>1133</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>492</v>
+        <v>1142</v>
       </c>
       <c r="F55" s="8" t="s">
-        <v>493</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="56" spans="1:6">
@@ -19086,16 +20047,16 @@
       </c>
       <c r="B56" s="12"/>
       <c r="C56" s="1" t="s">
-        <v>494</v>
+        <v>1124</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>495</v>
+        <v>1134</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>496</v>
+        <v>1143</v>
       </c>
       <c r="F56" s="8" t="s">
-        <v>494</v>
+        <v>1153</v>
       </c>
     </row>
     <row r="57" spans="1:6">
@@ -19104,16 +20065,16 @@
       </c>
       <c r="B57" s="12"/>
       <c r="C57" s="1" t="s">
-        <v>497</v>
+        <v>1125</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>498</v>
+        <v>1135</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>499</v>
+        <v>1144</v>
       </c>
       <c r="F57" s="8" t="s">
-        <v>500</v>
+        <v>1154</v>
       </c>
     </row>
     <row r="58" spans="1:6">
@@ -19140,16 +20101,16 @@
       </c>
       <c r="B59" s="12"/>
       <c r="C59" s="1" t="s">
-        <v>501</v>
+        <v>1126</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>502</v>
+        <v>1136</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>503</v>
+        <v>1145</v>
       </c>
       <c r="F59" s="8" t="s">
-        <v>504</v>
+        <v>1155</v>
       </c>
     </row>
     <row r="60" spans="1:6">
@@ -19158,16 +20119,16 @@
       </c>
       <c r="B60" s="12"/>
       <c r="C60" s="1" t="s">
-        <v>505</v>
+        <v>1127</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>506</v>
+        <v>1137</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>507</v>
+        <v>1146</v>
       </c>
       <c r="F60" s="8" t="s">
-        <v>508</v>
+        <v>1156</v>
       </c>
     </row>
     <row r="61" spans="1:6">
@@ -19178,16 +20139,16 @@
         <v>115</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>509</v>
+        <v>1128</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>510</v>
+        <v>1138</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>511</v>
+        <v>1147</v>
       </c>
       <c r="F61" s="8" t="s">
-        <v>512</v>
+        <v>1157</v>
       </c>
     </row>
     <row r="62" spans="1:6">
@@ -19196,16 +20157,16 @@
       </c>
       <c r="B62" s="12"/>
       <c r="C62" s="1" t="s">
-        <v>513</v>
+        <v>1129</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>514</v>
+        <v>1139</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>515</v>
+        <v>1148</v>
       </c>
       <c r="F62" s="8" t="s">
-        <v>516</v>
+        <v>1158</v>
       </c>
     </row>
     <row r="63" spans="1:6">
@@ -19214,16 +20175,16 @@
       </c>
       <c r="B63" s="12"/>
       <c r="C63" s="1" t="s">
-        <v>517</v>
+        <v>1130</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>518</v>
+        <v>1140</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>519</v>
+        <v>1149</v>
       </c>
       <c r="F63" s="8" t="s">
-        <v>520</v>
+        <v>1159</v>
       </c>
     </row>
     <row r="64" spans="1:6">
@@ -19232,16 +20193,16 @@
       </c>
       <c r="B64" s="12"/>
       <c r="C64" s="1" t="s">
-        <v>521</v>
+        <v>1131</v>
       </c>
       <c r="D64" s="1" t="s">
         <v>522</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>523</v>
+        <v>1150</v>
       </c>
       <c r="F64" s="8" t="s">
-        <v>524</v>
+        <v>1131</v>
       </c>
     </row>
     <row r="65" spans="1:6">
@@ -19337,14 +20298,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="39" t="s">
         <v>238</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="2" t="s">
@@ -20236,14 +21197,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="39" t="s">
         <v>279</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="2" t="s">
@@ -20508,14 +21469,14 @@
       <c r="F26" s="1"/>
     </row>
     <row r="29" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A29" s="39" t="s">
+      <c r="A29" s="40" t="s">
         <v>242</v>
       </c>
-      <c r="B29" s="40"/>
-      <c r="C29" s="40"/>
-      <c r="D29" s="40"/>
-      <c r="E29" s="40"/>
-      <c r="F29" s="41"/>
+      <c r="B29" s="41"/>
+      <c r="C29" s="41"/>
+      <c r="D29" s="41"/>
+      <c r="E29" s="41"/>
+      <c r="F29" s="42"/>
     </row>
     <row r="30" spans="1:6" ht="15.75" thickTop="1">
       <c r="A30" s="7" t="s">
@@ -21136,14 +22097,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="39" t="s">
         <v>327</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="2" t="s">
@@ -21408,14 +22369,14 @@
       <c r="F26" s="1"/>
     </row>
     <row r="29" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A29" s="39" t="s">
+      <c r="A29" s="40" t="s">
         <v>281</v>
       </c>
-      <c r="B29" s="40"/>
-      <c r="C29" s="40"/>
-      <c r="D29" s="40"/>
-      <c r="E29" s="40"/>
-      <c r="F29" s="41"/>
+      <c r="B29" s="41"/>
+      <c r="C29" s="41"/>
+      <c r="D29" s="41"/>
+      <c r="E29" s="41"/>
+      <c r="F29" s="42"/>
     </row>
     <row r="30" spans="1:6" ht="15.75" thickTop="1">
       <c r="A30" s="7" t="s">
@@ -22036,14 +22997,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="39" t="s">
         <v>378</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="2" t="s">
@@ -22308,14 +23269,14 @@
       <c r="F26" s="1"/>
     </row>
     <row r="29" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A29" s="39" t="s">
+      <c r="A29" s="40" t="s">
         <v>328</v>
       </c>
-      <c r="B29" s="40"/>
-      <c r="C29" s="40"/>
-      <c r="D29" s="40"/>
-      <c r="E29" s="40"/>
-      <c r="F29" s="41"/>
+      <c r="B29" s="41"/>
+      <c r="C29" s="41"/>
+      <c r="D29" s="41"/>
+      <c r="E29" s="41"/>
+      <c r="F29" s="42"/>
     </row>
     <row r="30" spans="1:6" ht="15.75" thickTop="1">
       <c r="A30" s="7" t="s">
@@ -22937,14 +23898,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="39" t="s">
         <v>419</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="2" t="s">
@@ -23209,14 +24170,14 @@
       <c r="F26" s="1"/>
     </row>
     <row r="29" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A29" s="39" t="s">
+      <c r="A29" s="40" t="s">
         <v>379</v>
       </c>
-      <c r="B29" s="40"/>
-      <c r="C29" s="40"/>
-      <c r="D29" s="40"/>
-      <c r="E29" s="40"/>
-      <c r="F29" s="41"/>
+      <c r="B29" s="41"/>
+      <c r="C29" s="41"/>
+      <c r="D29" s="41"/>
+      <c r="E29" s="41"/>
+      <c r="F29" s="42"/>
     </row>
     <row r="30" spans="1:6" ht="15.75" thickTop="1">
       <c r="A30" s="7" t="s">
@@ -23837,14 +24798,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="39" t="s">
         <v>473</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="2" t="s">
@@ -24109,14 +25070,14 @@
       <c r="F26" s="1"/>
     </row>
     <row r="29" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A29" s="39" t="s">
+      <c r="A29" s="40" t="s">
         <v>423</v>
       </c>
-      <c r="B29" s="40"/>
-      <c r="C29" s="40"/>
-      <c r="D29" s="40"/>
-      <c r="E29" s="40"/>
-      <c r="F29" s="41"/>
+      <c r="B29" s="41"/>
+      <c r="C29" s="41"/>
+      <c r="D29" s="41"/>
+      <c r="E29" s="41"/>
+      <c r="F29" s="42"/>
     </row>
     <row r="30" spans="1:6" ht="15.75" thickTop="1">
       <c r="A30" s="7" t="s">
@@ -24735,14 +25696,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="39" t="s">
         <v>473</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="2" t="s">
@@ -25007,14 +25968,14 @@
       <c r="F26" s="1"/>
     </row>
     <row r="29" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A29" s="39" t="s">
+      <c r="A29" s="40" t="s">
         <v>475</v>
       </c>
-      <c r="B29" s="40"/>
-      <c r="C29" s="40"/>
-      <c r="D29" s="40"/>
-      <c r="E29" s="40"/>
-      <c r="F29" s="41"/>
+      <c r="B29" s="41"/>
+      <c r="C29" s="41"/>
+      <c r="D29" s="41"/>
+      <c r="E29" s="41"/>
+      <c r="F29" s="42"/>
     </row>
     <row r="30" spans="1:6" ht="15.75" thickTop="1">
       <c r="A30" s="7" t="s">

</xml_diff>